<commit_message>
Updated `special pins` document
</commit_message>
<xml_diff>
--- a/doc/special pins.xlsx
+++ b/doc/special pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device_32\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFCE975-D3B8-4AB2-99BC-A9C92B17C4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3CD101-8ABB-4872-85A2-5F1AD9963894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-4470" windowWidth="16440" windowHeight="28320" xr2:uid="{BEF8E616-E74D-4737-A27B-098992C948DD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="106">
   <si>
     <t>TC</t>
   </si>
@@ -44,12 +44,12 @@
     <t>TC ID</t>
   </si>
   <si>
+    <t>TC CH</t>
+  </si>
+  <si>
     <t>PD7</t>
   </si>
   <si>
-    <t>D11</t>
-  </si>
-  <si>
     <t>D5</t>
   </si>
   <si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Event handling</t>
-  </si>
-  <si>
-    <t>Timer/counter use</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -315,11 +312,49 @@
     <t>Periph</t>
   </si>
   <si>
-    <t>TC
-CH</t>
-  </si>
-  <si>
     <t>TCs without output: 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Interlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                 </t>
+  </si>
+  <si>
+    <t>Summary of special pins</t>
+  </si>
+  <si>
+    <t>Interlock heartbeat output</t>
+  </si>
+  <si>
+    <t>Interlock heartbeat sensor in</t>
+  </si>
+  <si>
+    <t>Burst output</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>Cy2 pin (interlocked)</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Cy3 pin (interlocked)</t>
+  </si>
+  <si>
+    <t>Cy5 pin (interlocked)</t>
+  </si>
+  <si>
+    <t>Cy7 pin (interlocked)</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Timers/counters in use</t>
   </si>
 </sst>
 </file>
@@ -358,7 +393,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -395,11 +430,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -417,6 +474,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -457,7 +520,7 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{82A72967-1F50-46EF-897F-7D70496207F3}" name="TC ID"/>
     <tableColumn id="2" xr3:uid="{832B2D19-680C-4766-8CD3-5B6791BC398E}" name="TC"/>
-    <tableColumn id="3" xr3:uid="{50D573C8-D8F1-4F13-816E-8110888EC4C4}" name="TC_x000a_CH"/>
+    <tableColumn id="3" xr3:uid="{50D573C8-D8F1-4F13-816E-8110888EC4C4}" name="TC CH"/>
     <tableColumn id="4" xr3:uid="{5EB33E76-542F-4579-8A09-3C196916D78A}" name="Type"/>
     <tableColumn id="5" xr3:uid="{918175A0-CEA8-4951-861B-69D38D918D58}" name="Signal"/>
     <tableColumn id="6" xr3:uid="{A8D98A22-5B99-46E3-8ABD-53E6E0C28670}" name="I/O Line"/>
@@ -765,16 +828,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA132A4B-B8A3-46A0-AA6F-0424522B4A55}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="3" width="6" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -791,7 +855,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -802,22 +866,22 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -838,16 +902,16 @@
         <v>TCLK</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -868,16 +932,16 @@
         <v>TCLK</v>
       </c>
       <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" t="s">
         <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -898,16 +962,16 @@
         <v>TCLK</v>
       </c>
       <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -928,7 +992,7 @@
         <v>TIOA</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -937,37 +1001,37 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="9">
         <f>_xlfn.NUMBERVALUE( RIGHT(E9, 1))</f>
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <f>QUOTIENT(A9,3)</f>
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <f>MOD(A9,3)</f>
         <v>0</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="9" t="str">
         <f>LEFT(E9,4)</f>
         <v>TIOB</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
+        <v>78</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -988,13 +1052,13 @@
         <v>TIOA</v>
       </c>
       <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1015,7 +1079,7 @@
         <v>TIOA</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -1024,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1045,7 +1109,7 @@
         <v>TIOB</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1054,7 +1118,7 @@
         <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1075,7 +1139,7 @@
         <v>TIOB</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -1084,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1105,16 +1169,16 @@
         <v>TCLK</v>
       </c>
       <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
         <v>40</v>
       </c>
-      <c r="F14" t="s">
-        <v>41</v>
-      </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1135,16 +1199,16 @@
         <v>TCLK</v>
       </c>
       <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="F15" t="s">
-        <v>43</v>
-      </c>
       <c r="G15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1165,16 +1229,16 @@
         <v>TCLK</v>
       </c>
       <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
         <v>44</v>
       </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
       <c r="G16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1195,13 +1259,13 @@
         <v>TIOA</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1222,13 +1286,13 @@
         <v>TIOA</v>
       </c>
       <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
         <v>46</v>
       </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1249,13 +1313,13 @@
         <v>TIOA</v>
       </c>
       <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
         <v>48</v>
       </c>
-      <c r="F19" t="s">
-        <v>49</v>
-      </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1276,13 +1340,13 @@
         <v>TIOA</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1303,13 +1367,13 @@
         <v>TIOA</v>
       </c>
       <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
         <v>51</v>
       </c>
-      <c r="F21" t="s">
-        <v>52</v>
-      </c>
       <c r="H21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1330,13 +1394,13 @@
         <v>TIOA</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1357,13 +1421,13 @@
         <v>TIOB</v>
       </c>
       <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s">
         <v>54</v>
       </c>
-      <c r="F23" t="s">
-        <v>55</v>
-      </c>
       <c r="H23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1384,13 +1448,13 @@
         <v>TIOB</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1411,13 +1475,13 @@
         <v>TIOB</v>
       </c>
       <c r="E25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
         <v>57</v>
       </c>
-      <c r="F25" t="s">
-        <v>58</v>
-      </c>
       <c r="H25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1438,13 +1502,13 @@
         <v>TIOB</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1465,13 +1529,13 @@
         <v>TIOB</v>
       </c>
       <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" t="s">
         <v>60</v>
       </c>
-      <c r="F27" t="s">
-        <v>61</v>
-      </c>
       <c r="H27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1492,13 +1556,13 @@
         <v>TIOB</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1519,13 +1583,13 @@
         <v>TCLK</v>
       </c>
       <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
         <v>63</v>
       </c>
-      <c r="F29" t="s">
-        <v>64</v>
-      </c>
       <c r="H29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1546,13 +1610,13 @@
         <v>TCLK</v>
       </c>
       <c r="E30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" t="s">
         <v>65</v>
       </c>
-      <c r="F30" t="s">
-        <v>66</v>
-      </c>
       <c r="H30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1573,46 +1637,46 @@
         <v>TCLK</v>
       </c>
       <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
         <v>67</v>
       </c>
-      <c r="F31" t="s">
-        <v>68</v>
-      </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="9">
         <f>_xlfn.NUMBERVALUE( RIGHT(E32, 1))</f>
         <v>6</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="9">
         <f>QUOTIENT(A32,3)</f>
         <v>2</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="9">
         <f>MOD(A32,3)</f>
         <v>0</v>
       </c>
-      <c r="D32" t="str">
+      <c r="D32" s="9" t="str">
         <f>LEFT(E32,4)</f>
         <v>TIOA</v>
       </c>
       <c r="E32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H32" t="s">
-        <v>28</v>
+      <c r="H32" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1633,7 +1697,7 @@
         <v>TIOA</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F33" t="s">
         <v>7</v>
@@ -1642,7 +1706,7 @@
         <v>6</v>
       </c>
       <c r="H33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1663,16 +1727,16 @@
         <v>TIOA</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="H34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1693,13 +1757,13 @@
         <v>TIOB</v>
       </c>
       <c r="E35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" t="s">
         <v>72</v>
       </c>
-      <c r="F35" t="s">
-        <v>73</v>
-      </c>
       <c r="H35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1720,13 +1784,13 @@
         <v>TIOB</v>
       </c>
       <c r="E36" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" t="s">
         <v>74</v>
       </c>
-      <c r="F36" t="s">
-        <v>75</v>
-      </c>
       <c r="H36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,7 +1811,7 @@
         <v>TIOB</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37" t="s">
         <v>13</v>
@@ -1756,18 +1820,17 @@
         <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>93</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1775,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1783,6 +1846,9 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1824,17 +1890,90 @@
         <v>6</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>